<commit_message>
Write Paths Audit Completed
</commit_message>
<xml_diff>
--- a/inv.xlsx
+++ b/inv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mega\newProjectFullStack\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D37AFF-310B-4972-A8FC-93A4BFEB4C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA488B87-725F-4940-A158-469E11F2B302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{05CFEF9F-9FF6-4261-845E-06B51509E5C1}"/>
   </bookViews>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957C8121-B3AB-4B3E-B6AE-C9F77402D662}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -975,10 +975,10 @@
         <v>19</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J11" s="2">
         <v>309415906</v>

</xml_diff>